<commit_message>
analysis of primary outcomes
</commit_message>
<xml_diff>
--- a/data/old_data/orv_models_review_ pilot_data_2.xlsx
+++ b/data/old_data/orv_models_review_ pilot_data_2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23628"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Azam\Downloads\Documents\orv_review_data_extraction_analysis\orv_review_data_analysis\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Azam\GitRepositories\orv_models_review\data\old_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6D1E918-D835-45B5-931F-AD14BD5D662D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6BA0D4F-066E-4326-96E5-B9C266969A68}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="a3JjBseHG7RFrBGAxVbznP" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="890" uniqueCount="305">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="893" uniqueCount="308">
   <si>
     <t>start</t>
   </si>
@@ -935,6 +935,15 @@
   </si>
   <si>
     <t>2020-10-30T22:43:12</t>
+  </si>
+  <si>
+    <t>Key</t>
+  </si>
+  <si>
+    <t>Red=excluded</t>
+  </si>
+  <si>
+    <t>The other colors were only used to shade the rows for distinction and discussion</t>
   </si>
 </sst>
 </file>
@@ -944,7 +953,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -952,8 +961,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -998,13 +1015,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="2"/>
+        <fgColor theme="0" tint="-0.34998626667073579"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.34998626667073579"/>
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1021,7 +1044,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
@@ -1039,6 +1062,8 @@
     <xf numFmtId="164" fontId="0" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1377,19 +1402,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AY26"/>
+  <dimension ref="A1:AY31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+    <sheetView tabSelected="1" topLeftCell="AJ1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection activeCell="O1" sqref="O1"/>
+      <selection pane="bottomLeft" activeCell="O14" sqref="A14:XFD14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="8" width="0" hidden="1" customWidth="1"/>
     <col min="9" max="9" width="84.85546875" customWidth="1"/>
-    <col min="10" max="10" width="16" hidden="1" customWidth="1"/>
-    <col min="11" max="11" width="43.5703125" hidden="1" customWidth="1"/>
-    <col min="12" max="12" width="16.42578125" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="16" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="43.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.42578125" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="65.7109375" customWidth="1"/>
     <col min="14" max="14" width="34.7109375" customWidth="1"/>
     <col min="15" max="15" width="24.42578125" bestFit="1" customWidth="1"/>
@@ -1575,211 +1602,211 @@
         <v>50</v>
       </c>
     </row>
-    <row r="2" spans="1:51" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="2" spans="1:51" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="15" t="s">
         <v>146</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="15" t="s">
         <v>147</v>
       </c>
-      <c r="I2" t="s">
+      <c r="I2" s="15" t="s">
         <v>148</v>
       </c>
-      <c r="J2">
+      <c r="J2" s="15">
         <v>2019</v>
       </c>
-      <c r="K2" t="s">
+      <c r="K2" s="15" t="s">
         <v>149</v>
       </c>
-      <c r="L2" t="s">
+      <c r="L2" s="15" t="s">
         <v>55</v>
       </c>
-      <c r="M2" t="s">
+      <c r="M2" s="15" t="s">
         <v>56</v>
       </c>
-      <c r="N2" t="s">
+      <c r="N2" s="15" t="s">
         <v>150</v>
       </c>
-      <c r="Q2" t="s">
-        <v>78</v>
-      </c>
-      <c r="R2" t="s">
+      <c r="Q2" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="R2" s="15" t="s">
         <v>151</v>
       </c>
-      <c r="S2" t="s">
+      <c r="S2" s="15" t="s">
         <v>137</v>
       </c>
-      <c r="U2" t="s">
+      <c r="U2" s="15" t="s">
         <v>109</v>
       </c>
-      <c r="W2" t="s">
-        <v>58</v>
-      </c>
-      <c r="X2" t="s">
+      <c r="W2" s="15" t="s">
+        <v>58</v>
+      </c>
+      <c r="X2" s="15" t="s">
         <v>62</v>
       </c>
-      <c r="Z2" t="s">
+      <c r="Z2" s="15" t="s">
         <v>152</v>
       </c>
-      <c r="AA2" t="s">
+      <c r="AA2" s="15" t="s">
         <v>64</v>
       </c>
-      <c r="AC2" t="s">
+      <c r="AC2" s="15" t="s">
         <v>65</v>
       </c>
-      <c r="AD2" t="s">
+      <c r="AD2" s="15" t="s">
         <v>110</v>
       </c>
-      <c r="AF2" t="s">
-        <v>58</v>
-      </c>
-      <c r="AH2" t="s">
+      <c r="AF2" s="15" t="s">
+        <v>58</v>
+      </c>
+      <c r="AH2" s="15" t="s">
         <v>153</v>
       </c>
-      <c r="AI2" t="s">
+      <c r="AI2" s="15" t="s">
         <v>111</v>
       </c>
-      <c r="AK2" t="s">
-        <v>58</v>
-      </c>
-      <c r="AL2" t="s">
-        <v>78</v>
-      </c>
-      <c r="AM2" t="s">
-        <v>78</v>
-      </c>
-      <c r="AN2" t="s">
-        <v>78</v>
-      </c>
-      <c r="AO2" t="s">
+      <c r="AK2" s="15" t="s">
+        <v>58</v>
+      </c>
+      <c r="AL2" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="AM2" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="AN2" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="AO2" s="15" t="s">
         <v>69</v>
       </c>
-      <c r="AQ2" t="s">
+      <c r="AQ2" s="15" t="s">
         <v>154</v>
       </c>
-      <c r="AR2">
+      <c r="AR2" s="15">
         <v>71235777</v>
       </c>
-      <c r="AS2" t="s">
+      <c r="AS2" s="15" t="s">
         <v>155</v>
       </c>
-      <c r="AT2" t="s">
+      <c r="AT2" s="15" t="s">
         <v>156</v>
       </c>
-      <c r="AU2">
+      <c r="AU2" s="15">
         <v>8</v>
       </c>
-      <c r="AW2">
+      <c r="AW2" s="15">
         <v>-1</v>
       </c>
-      <c r="AX2" t="s">
-        <v>73</v>
-      </c>
-      <c r="AY2" t="s">
+      <c r="AX2" s="15" t="s">
+        <v>73</v>
+      </c>
+      <c r="AY2" s="15" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="3" spans="1:51" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="3" spans="1:51" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="15" t="s">
         <v>201</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="15" t="s">
         <v>202</v>
       </c>
-      <c r="I3" t="s">
+      <c r="I3" s="15" t="s">
         <v>203</v>
       </c>
-      <c r="J3">
+      <c r="J3" s="15">
         <v>2001</v>
       </c>
-      <c r="K3" t="s">
+      <c r="K3" s="15" t="s">
         <v>204</v>
       </c>
-      <c r="L3" t="s">
+      <c r="L3" s="15" t="s">
         <v>55</v>
       </c>
-      <c r="M3" t="s">
+      <c r="M3" s="15" t="s">
         <v>205</v>
       </c>
-      <c r="N3" t="s">
+      <c r="N3" s="15" t="s">
         <v>206</v>
       </c>
-      <c r="Q3" t="s">
-        <v>58</v>
-      </c>
-      <c r="R3" t="s">
+      <c r="Q3" s="15" t="s">
+        <v>58</v>
+      </c>
+      <c r="R3" s="15" t="s">
         <v>207</v>
       </c>
-      <c r="S3" t="s">
+      <c r="S3" s="15" t="s">
         <v>137</v>
       </c>
-      <c r="U3" t="s">
+      <c r="U3" s="15" t="s">
         <v>61</v>
       </c>
-      <c r="W3" t="s">
-        <v>58</v>
-      </c>
-      <c r="X3" t="s">
+      <c r="W3" s="15" t="s">
+        <v>58</v>
+      </c>
+      <c r="X3" s="15" t="s">
         <v>175</v>
       </c>
-      <c r="Z3" t="s">
+      <c r="Z3" s="15" t="s">
         <v>128</v>
       </c>
-      <c r="AA3" t="s">
+      <c r="AA3" s="15" t="s">
         <v>208</v>
       </c>
-      <c r="AC3" t="s">
+      <c r="AC3" s="15" t="s">
         <v>195</v>
       </c>
-      <c r="AD3" t="s">
+      <c r="AD3" s="15" t="s">
         <v>110</v>
       </c>
-      <c r="AF3" t="s">
-        <v>58</v>
-      </c>
-      <c r="AH3" t="s">
+      <c r="AF3" s="15" t="s">
+        <v>58</v>
+      </c>
+      <c r="AH3" s="15" t="s">
         <v>196</v>
       </c>
-      <c r="AI3" t="s">
+      <c r="AI3" s="15" t="s">
         <v>209</v>
       </c>
-      <c r="AK3" t="s">
-        <v>78</v>
-      </c>
-      <c r="AL3" t="s">
-        <v>78</v>
-      </c>
-      <c r="AM3" t="s">
-        <v>58</v>
-      </c>
-      <c r="AN3" t="s">
-        <v>58</v>
-      </c>
-      <c r="AO3" t="s">
+      <c r="AK3" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="AL3" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="AM3" s="15" t="s">
+        <v>58</v>
+      </c>
+      <c r="AN3" s="15" t="s">
+        <v>58</v>
+      </c>
+      <c r="AO3" s="15" t="s">
         <v>69</v>
       </c>
-      <c r="AQ3" t="s">
+      <c r="AQ3" s="15" t="s">
         <v>210</v>
       </c>
-      <c r="AR3">
+      <c r="AR3" s="15">
         <v>71246012</v>
       </c>
-      <c r="AS3" t="s">
+      <c r="AS3" s="15" t="s">
         <v>211</v>
       </c>
-      <c r="AT3" t="s">
+      <c r="AT3" s="15" t="s">
         <v>212</v>
       </c>
-      <c r="AU3">
+      <c r="AU3" s="15">
         <v>13</v>
       </c>
-      <c r="AW3">
+      <c r="AW3" s="15">
         <v>-1</v>
       </c>
-      <c r="AX3" t="s">
-        <v>73</v>
-      </c>
-      <c r="AY3" t="s">
+      <c r="AX3" s="15" t="s">
+        <v>73</v>
+      </c>
+      <c r="AY3" s="15" t="s">
         <v>73</v>
       </c>
     </row>
@@ -2473,125 +2500,125 @@
         <v>73</v>
       </c>
     </row>
-    <row r="10" spans="1:51" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
+    <row r="10" spans="1:51" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="B10" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="C10" s="4">
+      <c r="C10" s="2">
         <v>44125</v>
       </c>
-      <c r="D10" s="3" t="s">
+      <c r="D10" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="E10" s="3" t="s">
+      <c r="E10" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="F10" s="3" t="s">
+      <c r="F10" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="G10" s="3" t="s">
+      <c r="G10" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="H10" s="3" t="s">
+      <c r="H10" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="I10" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="J10" s="3">
+      <c r="I10" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="J10" s="1">
         <v>2014</v>
       </c>
-      <c r="K10" s="3" t="s">
+      <c r="K10" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="L10" s="3" t="s">
+      <c r="L10" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="M10" s="3" t="s">
+      <c r="M10" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="N10" s="3" t="s">
+      <c r="N10" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="Q10" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="R10" s="3" t="s">
+      <c r="Q10" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="R10" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="S10" s="3" t="s">
+      <c r="S10" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="U10" s="3" t="s">
+      <c r="U10" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="W10" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="X10" s="3" t="s">
+      <c r="W10" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="X10" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="Z10" s="3" t="s">
+      <c r="Z10" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="AA10" s="3" t="s">
+      <c r="AA10" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="AC10" s="3" t="s">
+      <c r="AC10" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="AD10" s="3" t="s">
+      <c r="AD10" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="AF10" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="AH10" s="3" t="s">
+      <c r="AF10" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="AH10" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="AI10" s="3" t="s">
+      <c r="AI10" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="AK10" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="AL10" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="AN10" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="AO10" s="3" t="s">
+      <c r="AK10" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="AL10" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="AN10" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="AO10" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="AP10" s="3" t="s">
+      <c r="AP10" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="AQ10" s="3" t="s">
+      <c r="AQ10" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="AR10" s="3">
+      <c r="AR10" s="1">
         <v>71178994</v>
       </c>
-      <c r="AS10" s="3" t="s">
+      <c r="AS10" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="AT10" s="3" t="s">
+      <c r="AT10" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="AU10" s="3">
+      <c r="AU10" s="1">
         <v>4</v>
       </c>
-      <c r="AW10" s="3">
+      <c r="AW10" s="1">
         <v>-1</v>
       </c>
-      <c r="AX10" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="AY10" s="3" t="s">
+      <c r="AX10" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="AY10" s="1" t="s">
         <v>73</v>
       </c>
     </row>
@@ -2821,104 +2848,104 @@
         <v>73</v>
       </c>
     </row>
-    <row r="13" spans="1:51" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="7" t="s">
+    <row r="13" spans="1:51" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="B13" s="7" t="s">
+      <c r="B13" s="3" t="s">
         <v>124</v>
       </c>
-      <c r="I13" s="7" t="s">
-        <v>125</v>
-      </c>
-      <c r="J13" s="7">
+      <c r="I13" s="3" t="s">
+        <v>264</v>
+      </c>
+      <c r="J13" s="3">
         <v>2016</v>
       </c>
-      <c r="K13" s="7" t="s">
+      <c r="K13" s="3" t="s">
         <v>126</v>
       </c>
-      <c r="L13" s="7" t="s">
+      <c r="L13" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="M13" s="7" t="s">
+      <c r="M13" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="N13" s="7" t="s">
+      <c r="N13" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="Q13" s="7" t="s">
-        <v>78</v>
-      </c>
-      <c r="R13" s="7" t="s">
+      <c r="Q13" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="R13" s="3" t="s">
         <v>127</v>
       </c>
-      <c r="S13" s="7" t="s">
+      <c r="S13" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="U13" s="7" t="s">
+      <c r="U13" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="W13" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="X13" s="7" t="s">
+      <c r="W13" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="X13" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="Z13" s="7" t="s">
+      <c r="Z13" s="3" t="s">
         <v>128</v>
       </c>
-      <c r="AA13" s="7" t="s">
+      <c r="AA13" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="AC13" s="7" t="s">
+      <c r="AC13" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="AD13" s="7" t="s">
+      <c r="AD13" s="3" t="s">
         <v>129</v>
       </c>
-      <c r="AF13" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="AH13" s="7" t="s">
+      <c r="AF13" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AH13" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="AI13" s="7" t="s">
+      <c r="AI13" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="AK13" s="7" t="s">
-        <v>78</v>
-      </c>
-      <c r="AL13" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="AN13" s="7" t="s">
-        <v>78</v>
-      </c>
-      <c r="AO13" s="7" t="s">
+      <c r="AK13" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="AL13" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AN13" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="AO13" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="AQ13" s="7" t="s">
+      <c r="AQ13" s="3" t="s">
         <v>131</v>
       </c>
-      <c r="AR13" s="7">
+      <c r="AR13" s="3">
         <v>71123539</v>
       </c>
-      <c r="AS13" s="7" t="s">
+      <c r="AS13" s="3" t="s">
         <v>132</v>
       </c>
-      <c r="AT13" s="7" t="s">
+      <c r="AT13" s="3" t="s">
         <v>133</v>
       </c>
-      <c r="AU13" s="7">
+      <c r="AU13" s="3">
         <v>6</v>
       </c>
-      <c r="AW13" s="7">
+      <c r="AW13" s="3">
         <v>-1</v>
       </c>
-      <c r="AX13" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="AY13" s="7" t="s">
+      <c r="AX13" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="AY13" s="3" t="s">
         <v>73</v>
       </c>
     </row>
@@ -3910,581 +3937,596 @@
         <v>73</v>
       </c>
     </row>
-    <row r="22" spans="1:51" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="13" t="s">
+    <row r="22" spans="1:51" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="15" t="s">
         <v>157</v>
       </c>
-      <c r="B22" s="13" t="s">
+      <c r="B22" s="15" t="s">
         <v>158</v>
       </c>
-      <c r="I22" s="13" t="s">
+      <c r="I22" s="15" t="s">
         <v>159</v>
       </c>
-      <c r="J22" s="13">
+      <c r="J22" s="15">
         <v>2018</v>
       </c>
-      <c r="K22" s="13" t="s">
+      <c r="K22" s="15" t="s">
         <v>160</v>
       </c>
-      <c r="L22" s="13" t="s">
+      <c r="L22" s="15" t="s">
         <v>55</v>
       </c>
-      <c r="M22" s="13" t="s">
+      <c r="M22" s="15" t="s">
         <v>56</v>
       </c>
-      <c r="N22" s="13" t="s">
+      <c r="N22" s="15" t="s">
         <v>161</v>
       </c>
-      <c r="Q22" s="13" t="s">
-        <v>78</v>
-      </c>
-      <c r="R22" s="13" t="s">
+      <c r="Q22" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="R22" s="15" t="s">
         <v>162</v>
       </c>
-      <c r="S22" s="13" t="s">
+      <c r="S22" s="15" t="s">
         <v>60</v>
       </c>
-      <c r="U22" s="13" t="s">
+      <c r="U22" s="15" t="s">
         <v>109</v>
       </c>
-      <c r="W22" s="13" t="s">
-        <v>58</v>
-      </c>
-      <c r="X22" s="13" t="s">
+      <c r="W22" s="15" t="s">
+        <v>58</v>
+      </c>
+      <c r="X22" s="15" t="s">
         <v>62</v>
       </c>
-      <c r="Z22" s="13" t="s">
+      <c r="Z22" s="15" t="s">
         <v>63</v>
       </c>
-      <c r="AA22" s="13" t="s">
+      <c r="AA22" s="15" t="s">
         <v>64</v>
       </c>
-      <c r="AC22" s="13" t="s">
+      <c r="AC22" s="15" t="s">
         <v>65</v>
       </c>
-      <c r="AD22" s="13" t="s">
+      <c r="AD22" s="15" t="s">
         <v>163</v>
       </c>
-      <c r="AE22" s="13" t="s">
+      <c r="AE22" s="15" t="s">
         <v>164</v>
       </c>
-      <c r="AF22" s="13" t="s">
-        <v>58</v>
-      </c>
-      <c r="AH22" s="13" t="s">
+      <c r="AF22" s="15" t="s">
+        <v>58</v>
+      </c>
+      <c r="AH22" s="15" t="s">
         <v>67</v>
       </c>
-      <c r="AI22" s="13" t="s">
+      <c r="AI22" s="15" t="s">
         <v>165</v>
       </c>
-      <c r="AK22" s="13" t="s">
-        <v>58</v>
-      </c>
-      <c r="AL22" s="13" t="s">
-        <v>58</v>
-      </c>
-      <c r="AN22" s="13" t="s">
-        <v>58</v>
-      </c>
-      <c r="AO22" s="13" t="s">
+      <c r="AK22" s="15" t="s">
+        <v>58</v>
+      </c>
+      <c r="AL22" s="15" t="s">
+        <v>58</v>
+      </c>
+      <c r="AN22" s="15" t="s">
+        <v>58</v>
+      </c>
+      <c r="AO22" s="15" t="s">
         <v>69</v>
       </c>
-      <c r="AQ22" s="13" t="s">
+      <c r="AQ22" s="15" t="s">
         <v>166</v>
       </c>
-      <c r="AR22" s="13">
+      <c r="AR22" s="15">
         <v>71237525</v>
       </c>
-      <c r="AS22" s="13" t="s">
+      <c r="AS22" s="15" t="s">
         <v>167</v>
       </c>
-      <c r="AT22" s="13" t="s">
+      <c r="AT22" s="15" t="s">
         <v>168</v>
       </c>
-      <c r="AU22" s="13">
+      <c r="AU22" s="15">
         <v>9</v>
       </c>
-      <c r="AW22" s="13">
+      <c r="AW22" s="15">
         <v>-1</v>
       </c>
-      <c r="AX22" s="13" t="s">
-        <v>73</v>
-      </c>
-      <c r="AY22" s="13" t="s">
+      <c r="AX22" s="15" t="s">
+        <v>73</v>
+      </c>
+      <c r="AY22" s="15" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="23" spans="1:51" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="13" t="s">
+    <row r="23" spans="1:51" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="15" t="s">
         <v>254</v>
       </c>
-      <c r="B23" s="13" t="s">
+      <c r="B23" s="15" t="s">
         <v>255</v>
       </c>
-      <c r="C23" s="14">
+      <c r="C23" s="16">
         <v>44125</v>
       </c>
-      <c r="D23" s="13" t="s">
+      <c r="D23" s="15" t="s">
         <v>87</v>
       </c>
-      <c r="E23" s="13" t="s">
+      <c r="E23" s="15" t="s">
         <v>88</v>
       </c>
-      <c r="F23" s="13" t="s">
+      <c r="F23" s="15" t="s">
         <v>89</v>
       </c>
-      <c r="G23" s="13" t="s">
+      <c r="G23" s="15" t="s">
         <v>90</v>
       </c>
-      <c r="H23" s="13" t="s">
+      <c r="H23" s="15" t="s">
         <v>91</v>
       </c>
-      <c r="I23" s="13" t="s">
+      <c r="I23" s="15" t="s">
         <v>159</v>
       </c>
-      <c r="J23" s="13">
+      <c r="J23" s="15">
         <v>2018</v>
       </c>
-      <c r="K23" s="13" t="s">
+      <c r="K23" s="15" t="s">
         <v>160</v>
       </c>
-      <c r="L23" s="13" t="s">
+      <c r="L23" s="15" t="s">
         <v>55</v>
       </c>
-      <c r="M23" s="13" t="s">
+      <c r="M23" s="15" t="s">
         <v>77</v>
       </c>
-      <c r="N23" s="13" t="s">
+      <c r="N23" s="15" t="s">
         <v>107</v>
       </c>
-      <c r="Q23" s="13" t="s">
-        <v>58</v>
-      </c>
-      <c r="R23" s="13" t="s">
+      <c r="Q23" s="15" t="s">
+        <v>58</v>
+      </c>
+      <c r="R23" s="15" t="s">
         <v>162</v>
       </c>
-      <c r="S23" s="13" t="s">
+      <c r="S23" s="15" t="s">
         <v>60</v>
       </c>
-      <c r="U23" s="13" t="s">
+      <c r="U23" s="15" t="s">
         <v>109</v>
       </c>
-      <c r="W23" s="13" t="s">
-        <v>58</v>
-      </c>
-      <c r="X23" s="13" t="s">
+      <c r="W23" s="15" t="s">
+        <v>58</v>
+      </c>
+      <c r="X23" s="15" t="s">
         <v>175</v>
       </c>
-      <c r="Z23" s="13" t="s">
+      <c r="Z23" s="15" t="s">
         <v>63</v>
       </c>
-      <c r="AA23" s="13" t="s">
+      <c r="AA23" s="15" t="s">
         <v>64</v>
       </c>
-      <c r="AC23" s="13" t="s">
+      <c r="AC23" s="15" t="s">
         <v>65</v>
       </c>
-      <c r="AD23" s="13" t="s">
+      <c r="AD23" s="15" t="s">
         <v>163</v>
       </c>
-      <c r="AE23" s="13" t="s">
+      <c r="AE23" s="15" t="s">
         <v>256</v>
       </c>
-      <c r="AF23" s="13" t="s">
-        <v>58</v>
-      </c>
-      <c r="AH23" s="13" t="s">
+      <c r="AF23" s="15" t="s">
+        <v>58</v>
+      </c>
+      <c r="AH23" s="15" t="s">
         <v>95</v>
       </c>
-      <c r="AI23" s="13" t="s">
+      <c r="AI23" s="15" t="s">
         <v>257</v>
       </c>
-      <c r="AK23" s="13" t="s">
-        <v>58</v>
-      </c>
-      <c r="AL23" s="13" t="s">
-        <v>58</v>
-      </c>
-      <c r="AN23" s="13" t="s">
-        <v>58</v>
-      </c>
-      <c r="AO23" s="13" t="s">
+      <c r="AK23" s="15" t="s">
+        <v>58</v>
+      </c>
+      <c r="AL23" s="15" t="s">
+        <v>58</v>
+      </c>
+      <c r="AN23" s="15" t="s">
+        <v>58</v>
+      </c>
+      <c r="AO23" s="15" t="s">
         <v>97</v>
       </c>
-      <c r="AP23" s="13" t="s">
+      <c r="AP23" s="15" t="s">
         <v>98</v>
       </c>
-      <c r="AQ23" s="13" t="s">
+      <c r="AQ23" s="15" t="s">
         <v>258</v>
       </c>
-      <c r="AR23" s="13">
+      <c r="AR23" s="15">
         <v>71315567</v>
       </c>
-      <c r="AS23" s="13" t="s">
+      <c r="AS23" s="15" t="s">
         <v>259</v>
       </c>
-      <c r="AT23" s="13" t="s">
+      <c r="AT23" s="15" t="s">
         <v>260</v>
       </c>
-      <c r="AU23" s="13">
+      <c r="AU23" s="15">
         <v>19</v>
       </c>
-      <c r="AW23" s="13">
+      <c r="AW23" s="15">
         <v>-1</v>
       </c>
-      <c r="AX23" s="13" t="s">
-        <v>73</v>
-      </c>
-      <c r="AY23" s="13" t="s">
+      <c r="AX23" s="15" t="s">
+        <v>73</v>
+      </c>
+      <c r="AY23" s="15" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="24" spans="1:51" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="15" t="s">
+    <row r="24" spans="1:51" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="13" t="s">
         <v>213</v>
       </c>
-      <c r="B24" s="15" t="s">
+      <c r="B24" s="13" t="s">
         <v>214</v>
       </c>
-      <c r="I24" s="15" t="s">
+      <c r="I24" s="13" t="s">
         <v>215</v>
       </c>
-      <c r="J24" s="15">
+      <c r="J24" s="13">
         <v>2007</v>
       </c>
-      <c r="K24" s="15" t="s">
+      <c r="K24" s="13" t="s">
         <v>216</v>
       </c>
-      <c r="L24" s="15" t="s">
+      <c r="L24" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="M24" s="15" t="s">
+      <c r="M24" s="13" t="s">
         <v>56</v>
       </c>
-      <c r="N24" s="15" t="s">
+      <c r="N24" s="13" t="s">
         <v>150</v>
       </c>
-      <c r="Q24" s="15" t="s">
-        <v>78</v>
-      </c>
-      <c r="R24" s="15" t="s">
+      <c r="Q24" s="13" t="s">
+        <v>78</v>
+      </c>
+      <c r="R24" s="13" t="s">
         <v>217</v>
       </c>
-      <c r="S24" s="15" t="s">
+      <c r="S24" s="13" t="s">
         <v>137</v>
       </c>
-      <c r="U24" s="15" t="s">
+      <c r="U24" s="13" t="s">
         <v>109</v>
       </c>
-      <c r="W24" s="15" t="s">
-        <v>58</v>
-      </c>
-      <c r="X24" s="15" t="s">
+      <c r="W24" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="X24" s="13" t="s">
         <v>175</v>
       </c>
-      <c r="Z24" s="15" t="s">
+      <c r="Z24" s="13" t="s">
         <v>63</v>
       </c>
-      <c r="AA24" s="15" t="s">
+      <c r="AA24" s="13" t="s">
         <v>64</v>
       </c>
-      <c r="AC24" s="15" t="s">
+      <c r="AC24" s="13" t="s">
         <v>65</v>
       </c>
-      <c r="AD24" s="15" t="s">
+      <c r="AD24" s="13" t="s">
         <v>110</v>
       </c>
-      <c r="AF24" s="15" t="s">
-        <v>58</v>
-      </c>
-      <c r="AH24" s="15" t="s">
+      <c r="AF24" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="AH24" s="13" t="s">
         <v>67</v>
       </c>
-      <c r="AI24" s="15" t="s">
+      <c r="AI24" s="13" t="s">
         <v>218</v>
       </c>
-      <c r="AK24" s="15" t="s">
-        <v>58</v>
-      </c>
-      <c r="AL24" s="15" t="s">
-        <v>58</v>
-      </c>
-      <c r="AN24" s="15" t="s">
-        <v>78</v>
-      </c>
-      <c r="AO24" s="15" t="s">
+      <c r="AK24" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="AL24" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="AN24" s="13" t="s">
+        <v>78</v>
+      </c>
+      <c r="AO24" s="13" t="s">
         <v>69</v>
       </c>
-      <c r="AQ24" s="15" t="s">
+      <c r="AQ24" s="13" t="s">
         <v>219</v>
       </c>
-      <c r="AR24" s="15">
+      <c r="AR24" s="13">
         <v>71247537</v>
       </c>
-      <c r="AS24" s="15" t="s">
+      <c r="AS24" s="13" t="s">
         <v>220</v>
       </c>
-      <c r="AT24" s="15" t="s">
+      <c r="AT24" s="13" t="s">
         <v>221</v>
       </c>
-      <c r="AU24" s="15">
+      <c r="AU24" s="13">
         <v>14</v>
       </c>
-      <c r="AW24" s="15">
+      <c r="AW24" s="13">
         <v>-1</v>
       </c>
-      <c r="AX24" s="15" t="s">
-        <v>73</v>
-      </c>
-      <c r="AY24" s="15" t="s">
+      <c r="AX24" s="13" t="s">
+        <v>73</v>
+      </c>
+      <c r="AY24" s="13" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="25" spans="1:51" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="15" t="s">
+    <row r="25" spans="1:51" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="13" t="s">
         <v>230</v>
       </c>
-      <c r="B25" s="15" t="s">
+      <c r="B25" s="13" t="s">
         <v>231</v>
       </c>
-      <c r="C25" s="16">
+      <c r="C25" s="14">
         <v>44125</v>
       </c>
-      <c r="D25" s="15" t="s">
+      <c r="D25" s="13" t="s">
         <v>87</v>
       </c>
-      <c r="E25" s="15" t="s">
+      <c r="E25" s="13" t="s">
         <v>88</v>
       </c>
-      <c r="F25" s="15" t="s">
+      <c r="F25" s="13" t="s">
         <v>89</v>
       </c>
-      <c r="G25" s="15" t="s">
+      <c r="G25" s="13" t="s">
         <v>90</v>
       </c>
-      <c r="H25" s="15" t="s">
+      <c r="H25" s="13" t="s">
         <v>91</v>
       </c>
-      <c r="I25" s="15" t="s">
+      <c r="I25" s="13" t="s">
         <v>215</v>
       </c>
-      <c r="J25" s="15">
+      <c r="J25" s="13">
         <v>2007</v>
       </c>
-      <c r="K25" s="15" t="s">
+      <c r="K25" s="13" t="s">
         <v>232</v>
       </c>
-      <c r="L25" s="15" t="s">
+      <c r="L25" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="M25" s="15" t="s">
+      <c r="M25" s="13" t="s">
         <v>77</v>
       </c>
-      <c r="N25" s="15" t="s">
+      <c r="N25" s="13" t="s">
         <v>150</v>
       </c>
-      <c r="Q25" s="15" t="s">
-        <v>78</v>
-      </c>
-      <c r="R25" s="15" t="s">
+      <c r="Q25" s="13" t="s">
+        <v>78</v>
+      </c>
+      <c r="R25" s="13" t="s">
         <v>217</v>
       </c>
-      <c r="S25" s="15" t="s">
+      <c r="S25" s="13" t="s">
         <v>60</v>
       </c>
-      <c r="U25" s="15" t="s">
+      <c r="U25" s="13" t="s">
         <v>109</v>
       </c>
-      <c r="W25" s="15" t="s">
-        <v>58</v>
-      </c>
-      <c r="X25" s="15" t="s">
+      <c r="W25" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="X25" s="13" t="s">
         <v>62</v>
       </c>
-      <c r="Z25" s="15" t="s">
+      <c r="Z25" s="13" t="s">
         <v>79</v>
       </c>
-      <c r="AA25" s="15" t="s">
+      <c r="AA25" s="13" t="s">
         <v>64</v>
       </c>
-      <c r="AC25" s="15" t="s">
+      <c r="AC25" s="13" t="s">
         <v>65</v>
       </c>
-      <c r="AD25" s="15" t="s">
+      <c r="AD25" s="13" t="s">
         <v>110</v>
       </c>
-      <c r="AF25" s="15" t="s">
-        <v>58</v>
-      </c>
-      <c r="AH25" s="15" t="s">
+      <c r="AF25" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="AH25" s="13" t="s">
         <v>95</v>
       </c>
-      <c r="AI25" s="15" t="s">
+      <c r="AI25" s="13" t="s">
         <v>225</v>
       </c>
-      <c r="AJ25" s="15" t="s">
+      <c r="AJ25" s="13" t="s">
         <v>233</v>
       </c>
-      <c r="AK25" s="15" t="s">
-        <v>58</v>
-      </c>
-      <c r="AL25" s="15" t="s">
-        <v>58</v>
-      </c>
-      <c r="AN25" s="15" t="s">
-        <v>58</v>
-      </c>
-      <c r="AO25" s="15" t="s">
+      <c r="AK25" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="AL25" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="AN25" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="AO25" s="13" t="s">
         <v>97</v>
       </c>
-      <c r="AP25" s="15" t="s">
+      <c r="AP25" s="13" t="s">
         <v>98</v>
       </c>
-      <c r="AQ25" s="15" t="s">
+      <c r="AQ25" s="13" t="s">
         <v>234</v>
       </c>
-      <c r="AR25" s="15">
+      <c r="AR25" s="13">
         <v>71302782</v>
       </c>
-      <c r="AS25" s="15" t="s">
+      <c r="AS25" s="13" t="s">
         <v>235</v>
       </c>
-      <c r="AT25" s="15" t="s">
+      <c r="AT25" s="13" t="s">
         <v>236</v>
       </c>
-      <c r="AU25" s="15">
+      <c r="AU25" s="13">
         <v>16</v>
       </c>
-      <c r="AW25" s="15">
+      <c r="AW25" s="13">
         <v>-1</v>
       </c>
-      <c r="AX25" s="15" t="s">
-        <v>73</v>
-      </c>
-      <c r="AY25" s="15" t="s">
+      <c r="AX25" s="13" t="s">
+        <v>73</v>
+      </c>
+      <c r="AY25" s="13" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="26" spans="1:51" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="15" t="s">
+    <row r="26" spans="1:51" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="13" t="s">
         <v>299</v>
       </c>
-      <c r="B26" s="15" t="s">
+      <c r="B26" s="13" t="s">
         <v>300</v>
       </c>
-      <c r="C26" s="16">
+      <c r="C26" s="14">
         <v>44135</v>
       </c>
-      <c r="D26" s="15" t="s">
+      <c r="D26" s="13" t="s">
         <v>87</v>
       </c>
-      <c r="E26" s="15" t="s">
+      <c r="E26" s="13" t="s">
         <v>88</v>
       </c>
-      <c r="F26" s="15" t="s">
+      <c r="F26" s="13" t="s">
         <v>89</v>
       </c>
-      <c r="G26" s="15" t="s">
+      <c r="G26" s="13" t="s">
         <v>263</v>
       </c>
-      <c r="H26" s="15" t="s">
+      <c r="H26" s="13" t="s">
         <v>91</v>
       </c>
-      <c r="I26" s="15" t="s">
+      <c r="I26" s="13" t="s">
         <v>215</v>
       </c>
-      <c r="J26" s="15">
+      <c r="J26" s="13">
         <v>2007</v>
       </c>
-      <c r="K26" s="15" t="s">
+      <c r="K26" s="13" t="s">
         <v>216</v>
       </c>
-      <c r="L26" s="15" t="s">
+      <c r="L26" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="M26" s="15" t="s">
+      <c r="M26" s="13" t="s">
         <v>106</v>
       </c>
-      <c r="N26" s="15" t="s">
+      <c r="N26" s="13" t="s">
         <v>150</v>
       </c>
-      <c r="Q26" s="15" t="s">
-        <v>78</v>
-      </c>
-      <c r="R26" s="15" t="s">
+      <c r="Q26" s="13" t="s">
+        <v>78</v>
+      </c>
+      <c r="R26" s="13" t="s">
         <v>217</v>
       </c>
-      <c r="S26" s="15" t="s">
+      <c r="S26" s="13" t="s">
         <v>60</v>
       </c>
-      <c r="U26" s="15" t="s">
+      <c r="U26" s="13" t="s">
         <v>109</v>
       </c>
-      <c r="W26" s="15" t="s">
-        <v>58</v>
-      </c>
-      <c r="X26" s="15" t="s">
+      <c r="W26" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="X26" s="13" t="s">
         <v>62</v>
       </c>
-      <c r="Z26" s="15" t="s">
+      <c r="Z26" s="13" t="s">
         <v>128</v>
       </c>
-      <c r="AA26" s="15" t="s">
+      <c r="AA26" s="13" t="s">
         <v>64</v>
       </c>
-      <c r="AC26" s="15" t="s">
+      <c r="AC26" s="13" t="s">
         <v>65</v>
       </c>
-      <c r="AD26" s="15" t="s">
+      <c r="AD26" s="13" t="s">
         <v>110</v>
       </c>
-      <c r="AF26" s="15" t="s">
-        <v>58</v>
-      </c>
-      <c r="AH26" s="15" t="s">
+      <c r="AF26" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="AH26" s="13" t="s">
         <v>95</v>
       </c>
-      <c r="AI26" s="15" t="s">
+      <c r="AI26" s="13" t="s">
         <v>301</v>
       </c>
-      <c r="AK26" s="15" t="s">
-        <v>58</v>
-      </c>
-      <c r="AL26" s="15" t="s">
-        <v>58</v>
-      </c>
-      <c r="AN26" s="15" t="s">
-        <v>58</v>
-      </c>
-      <c r="AO26" s="15" t="s">
+      <c r="AK26" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="AL26" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="AN26" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="AO26" s="13" t="s">
         <v>97</v>
       </c>
-      <c r="AP26" s="15" t="s">
+      <c r="AP26" s="13" t="s">
         <v>266</v>
       </c>
-      <c r="AQ26" s="15" t="s">
+      <c r="AQ26" s="13" t="s">
         <v>302</v>
       </c>
-      <c r="AR26" s="15">
+      <c r="AR26" s="13">
         <v>72443662</v>
       </c>
-      <c r="AS26" s="15" t="s">
+      <c r="AS26" s="13" t="s">
         <v>303</v>
       </c>
-      <c r="AT26" s="15" t="s">
+      <c r="AT26" s="13" t="s">
         <v>304</v>
       </c>
-      <c r="AU26" s="15">
+      <c r="AU26" s="13">
         <v>25</v>
       </c>
-      <c r="AW26" s="15">
+      <c r="AW26" s="13">
         <v>-1</v>
       </c>
-      <c r="AX26" s="15" t="s">
-        <v>73</v>
-      </c>
-      <c r="AY26" s="15" t="s">
-        <v>73</v>
+      <c r="AX26" s="13" t="s">
+        <v>73</v>
+      </c>
+      <c r="AY26" s="13" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="29" spans="1:51" x14ac:dyDescent="0.25">
+      <c r="I29" s="18" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="30" spans="1:51" x14ac:dyDescent="0.25">
+      <c r="I30" s="17" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="31" spans="1:51" x14ac:dyDescent="0.25">
+      <c r="I31" s="17" t="s">
+        <v>307</v>
       </c>
     </row>
   </sheetData>

</xml_diff>